<commit_message>
Refactor lms data augmentation
</commit_message>
<xml_diff>
--- a/results/pose_results_10_03_2021.xlsx
+++ b/results/pose_results_10_03_2021.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Pessa001/Desktop/pain_horses/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02172BFE-CB36-6345-9C6B-D47A9A4333E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F9905F-47CD-314E-BEC7-9C316C1BAF21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{E2B08CCA-CAB0-3A45-9B67-AAFB1F146EEB}"/>
+    <workbookView minimized="1" xWindow="14200" yWindow="-17540" windowWidth="19200" windowHeight="17540" xr2:uid="{E2B08CCA-CAB0-3A45-9B67-AAFB1F146EEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="cross validation 22 - 3 - 2021" sheetId="2" r:id="rId1"/>
+    <sheet name="10 - 3 - 2021" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="28">
   <si>
     <t>MAE</t>
   </si>
@@ -68,12 +69,63 @@
   <si>
     <t>Sheep + augmentation 0.7 - 50 epochs</t>
   </si>
+  <si>
+    <t xml:space="preserve">Transfer Learning: </t>
+  </si>
+  <si>
+    <t>hopenet_robust_alpha1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number epochs used: </t>
+  </si>
+  <si>
+    <t>MAE (on validation set)</t>
+  </si>
+  <si>
+    <t>PCC (on validation set)</t>
+  </si>
+  <si>
+    <t>hopenet_0_100_ep__best</t>
+  </si>
+  <si>
+    <t>hopenet_1_100_ep__best</t>
+  </si>
+  <si>
+    <t>hopenet_2_100_ep__best</t>
+  </si>
+  <si>
+    <t>Best epochs:</t>
+  </si>
+  <si>
+    <t>MAE (on test set)</t>
+  </si>
+  <si>
+    <t>PCC (on test set)</t>
+  </si>
+  <si>
+    <t>sheep_model</t>
+  </si>
+  <si>
+    <t>hopenet_sheep_ep_100_0__best</t>
+  </si>
+  <si>
+    <t>hopenet_sheep_ep_100_1__best</t>
+  </si>
+  <si>
+    <t>hopenet_sheep_ep_100_2__best</t>
+  </si>
+  <si>
+    <t>sheep_model with aug 0.7</t>
+  </si>
+  <si>
+    <t>sheep_model with aug 0.5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,8 +161,14 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +216,36 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,7 +266,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
@@ -191,6 +279,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -511,10 +609,1011 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB62F2C0-D72B-3A42-86A3-F9083901C0B1}">
+  <dimension ref="A1:J51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="10">
+        <v>100</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
+      <c r="B5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="10">
+        <v>11.7761</v>
+      </c>
+      <c r="C6" s="10">
+        <v>7.4326999999999996</v>
+      </c>
+      <c r="D6" s="10">
+        <v>4.0625</v>
+      </c>
+      <c r="E6" s="16">
+        <f>AVERAGE(B6:D6)</f>
+        <v>7.7571000000000003</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <v>0.3251</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.32979999999999998</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.1845</v>
+      </c>
+      <c r="J6" s="16">
+        <f>AVERAGE(G6:I6)</f>
+        <v>0.27979999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="10">
+        <v>16.419899999999998</v>
+      </c>
+      <c r="C7" s="10">
+        <v>11.704700000000001</v>
+      </c>
+      <c r="D7" s="10">
+        <v>7.9466000000000001</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" ref="E7:E8" si="0">AVERAGE(B7:D7)</f>
+        <v>12.023733333333334</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
+        <v>0.81159999999999999</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.7157</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="J7" s="16">
+        <f t="shared" ref="J7:J8" si="1">AVERAGE(G7:I7)</f>
+        <v>0.77576666666666672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="10">
+        <v>11.244</v>
+      </c>
+      <c r="C8" s="10">
+        <v>10.415900000000001</v>
+      </c>
+      <c r="D8" s="10">
+        <v>7.3148999999999997</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>9.6582666666666679</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.56640000000000001</v>
+      </c>
+      <c r="J8" s="16">
+        <f t="shared" si="1"/>
+        <v>0.67563333333333342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10"/>
+      <c r="B9" s="16">
+        <f>AVERAGE(B6:B8)</f>
+        <v>13.146666666666667</v>
+      </c>
+      <c r="C9" s="16">
+        <f t="shared" ref="C9:E9" si="2">AVERAGE(C6:C8)</f>
+        <v>9.8511000000000006</v>
+      </c>
+      <c r="D9" s="16">
+        <f t="shared" si="2"/>
+        <v>6.4413333333333327</v>
+      </c>
+      <c r="E9" s="16">
+        <f t="shared" si="2"/>
+        <v>9.8130333333333351</v>
+      </c>
+      <c r="G9" s="16">
+        <f>AVERAGE(G6:G8)</f>
+        <v>0.68773333333333342</v>
+      </c>
+      <c r="H9" s="16">
+        <f t="shared" ref="H9:J9" si="3">AVERAGE(H6:H8)</f>
+        <v>0.52650000000000008</v>
+      </c>
+      <c r="I9" s="16">
+        <f t="shared" si="3"/>
+        <v>0.51696666666666669</v>
+      </c>
+      <c r="J9" s="16">
+        <f t="shared" si="3"/>
+        <v>0.57706666666666673</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="10"/>
+      <c r="B10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="e">
+        <f>AVERAGE(B12:D12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10" t="e">
+        <f>AVERAGE(G12:I12)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="10">
+        <v>100</v>
+      </c>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="10"/>
+      <c r="B18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="10"/>
+      <c r="B19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="10">
+        <v>9.6350999999999996</v>
+      </c>
+      <c r="C20" s="10">
+        <v>5.8029000000000002</v>
+      </c>
+      <c r="D20" s="10">
+        <v>3.113</v>
+      </c>
+      <c r="E20" s="16">
+        <f>AVERAGE(B20:D20)</f>
+        <v>6.1836666666666664</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10">
+        <v>0.3009</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.60609999999999997</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0.39539999999999997</v>
+      </c>
+      <c r="J20" s="16">
+        <f>AVERAGE(G20:I20)</f>
+        <v>0.43413333333333332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="10">
+        <v>7.6848000000000001</v>
+      </c>
+      <c r="C21" s="10">
+        <v>7.7874999999999996</v>
+      </c>
+      <c r="D21" s="10">
+        <v>5.3296999999999999</v>
+      </c>
+      <c r="E21" s="16">
+        <f t="shared" ref="E21:E22" si="4">AVERAGE(B21:D21)</f>
+        <v>6.9340000000000002</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10">
+        <v>0.96650000000000003</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.74490000000000001</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0.81030000000000002</v>
+      </c>
+      <c r="J21" s="16">
+        <f t="shared" ref="J21:J22" si="5">AVERAGE(G21:I21)</f>
+        <v>0.84056666666666668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="10">
+        <v>12.561299999999999</v>
+      </c>
+      <c r="C22" s="10">
+        <v>10.5665</v>
+      </c>
+      <c r="D22" s="10">
+        <v>7.4179000000000004</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="4"/>
+        <v>10.181900000000001</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10">
+        <v>0.90669999999999995</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0.44450000000000001</v>
+      </c>
+      <c r="I22" s="10">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="J22" s="16">
+        <f t="shared" si="5"/>
+        <v>0.57973333333333332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="10"/>
+      <c r="B23" s="16">
+        <f>AVERAGE(B20:B22)</f>
+        <v>9.9603999999999999</v>
+      </c>
+      <c r="C23" s="16">
+        <f t="shared" ref="C23:E23" si="6">AVERAGE(C20:C22)</f>
+        <v>8.0523000000000007</v>
+      </c>
+      <c r="D23" s="16">
+        <f t="shared" si="6"/>
+        <v>5.2868666666666675</v>
+      </c>
+      <c r="E23" s="16">
+        <f t="shared" si="6"/>
+        <v>7.7665222222222221</v>
+      </c>
+      <c r="G23" s="16">
+        <f>AVERAGE(G20:G22)</f>
+        <v>0.72470000000000001</v>
+      </c>
+      <c r="H23" s="16">
+        <f>AVERAGE(H20:H22)</f>
+        <v>0.59850000000000003</v>
+      </c>
+      <c r="I23" s="16">
+        <f>AVERAGE(I20:I22)</f>
+        <v>0.53123333333333334</v>
+      </c>
+      <c r="J23" s="17">
+        <f>AVERAGE(J20:J22)</f>
+        <v>0.61814444444444439</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="10"/>
+      <c r="B24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="10">
+        <v>100</v>
+      </c>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="10"/>
+      <c r="B31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="10"/>
+      <c r="B32" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="B33" s="10">
+        <v>6.3723999999999998</v>
+      </c>
+      <c r="C33" s="10">
+        <v>5.2942999999999998</v>
+      </c>
+      <c r="D33" s="10">
+        <v>2.8437999999999999</v>
+      </c>
+      <c r="E33" s="16">
+        <f>AVERAGE(B33:D33)</f>
+        <v>4.8368333333333329</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0.74209999999999998</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0.48709999999999998</v>
+      </c>
+      <c r="J33" s="16">
+        <f t="shared" ref="J33:J35" si="7">AVERAGE(G33:I33)</f>
+        <v>0.41389999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="11"/>
+      <c r="B34">
+        <v>1.9883</v>
+      </c>
+      <c r="C34">
+        <v>2.2397</v>
+      </c>
+      <c r="D34">
+        <v>1.6781999999999999</v>
+      </c>
+      <c r="E34" s="16">
+        <f t="shared" ref="E34:E35" si="8">AVERAGE(B34:D34)</f>
+        <v>1.9687333333333334</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10">
+        <v>0.99809999999999999</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0.99239999999999995</v>
+      </c>
+      <c r="J34" s="16">
+        <f t="shared" si="7"/>
+        <v>0.99183333333333323</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="10">
+        <v>1.9420999999999999</v>
+      </c>
+      <c r="C35" s="10">
+        <v>2.4058999999999999</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1.9225000000000001</v>
+      </c>
+      <c r="E35" s="16">
+        <f t="shared" si="8"/>
+        <v>2.0901666666666667</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10">
+        <v>0.99870000000000003</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="I35" s="10">
+        <v>0.96689999999999998</v>
+      </c>
+      <c r="J35" s="16">
+        <f t="shared" si="7"/>
+        <v>0.97820000000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="10"/>
+      <c r="B36" s="16">
+        <f>AVERAGE(B33:B35)</f>
+        <v>3.4342666666666664</v>
+      </c>
+      <c r="C36" s="16">
+        <f t="shared" ref="C36:E36" si="9">AVERAGE(C33:C35)</f>
+        <v>3.3132999999999999</v>
+      </c>
+      <c r="D36" s="16">
+        <f t="shared" si="9"/>
+        <v>2.148166666666667</v>
+      </c>
+      <c r="E36" s="16">
+        <f t="shared" si="9"/>
+        <v>2.9652444444444441</v>
+      </c>
+      <c r="G36" s="16">
+        <f>AVERAGE(G33:G35)</f>
+        <v>0.66976666666666673</v>
+      </c>
+      <c r="H36" s="16">
+        <f t="shared" ref="H36:J36" si="10">AVERAGE(H33:H35)</f>
+        <v>0.89869999999999994</v>
+      </c>
+      <c r="I36" s="16">
+        <f t="shared" si="10"/>
+        <v>0.81546666666666656</v>
+      </c>
+      <c r="J36" s="16">
+        <f t="shared" si="10"/>
+        <v>0.79464444444444438</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="10"/>
+      <c r="B37" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="10"/>
+      <c r="B38" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="10">
+        <v>100</v>
+      </c>
+      <c r="C42" s="10"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="10"/>
+      <c r="B44" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="10"/>
+      <c r="B45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="10">
+        <v>1.8533999999999999</v>
+      </c>
+      <c r="C46" s="10">
+        <v>2.2170999999999998</v>
+      </c>
+      <c r="D46" s="10">
+        <v>1.6244000000000001</v>
+      </c>
+      <c r="E46" s="16">
+        <v>1.8983000000000001</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10">
+        <v>0.99839999999999995</v>
+      </c>
+      <c r="H46" s="10">
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="I46" s="10">
+        <v>0.99639999999999995</v>
+      </c>
+      <c r="J46" s="16"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="11"/>
+      <c r="B47">
+        <v>2.1213000000000002</v>
+      </c>
+      <c r="C47">
+        <v>2.3121999999999998</v>
+      </c>
+      <c r="D47">
+        <v>1.8936999999999999</v>
+      </c>
+      <c r="E47" s="16">
+        <v>2.109</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10">
+        <v>0.998</v>
+      </c>
+      <c r="H47" s="10">
+        <v>0.97770000000000001</v>
+      </c>
+      <c r="I47" s="10">
+        <v>0.96430000000000005</v>
+      </c>
+      <c r="J47" s="16"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="11"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="16"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="10"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="10"/>
+      <c r="B50" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="10"/>
+      <c r="B51" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="10"/>
+      <c r="G51" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="G10:J10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04671CCD-B35C-354B-B0EC-4D2462F4661A}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -638,7 +1737,7 @@
       </c>
       <c r="M4" s="1"/>
       <c r="N4">
-        <f t="shared" ref="N3:N20" si="1">AVERAGE(J4:L4)</f>
+        <f t="shared" ref="N4:N5" si="1">AVERAGE(J4:L4)</f>
         <v>0.46379999999999999</v>
       </c>
     </row>
@@ -754,7 +1853,7 @@
       </c>
       <c r="M8" s="1"/>
       <c r="N8">
-        <f t="shared" ref="N8:N20" si="2">AVERAGE(J8:L8)</f>
+        <f t="shared" ref="N8:N10" si="2">AVERAGE(J8:L8)</f>
         <v>10.4991</v>
       </c>
     </row>
@@ -896,7 +1995,7 @@
       </c>
       <c r="M13" s="1"/>
       <c r="N13">
-        <f t="shared" ref="N13:N20" si="3">AVERAGE(J13:L13)</f>
+        <f t="shared" ref="N13:N15" si="3">AVERAGE(J13:L13)</f>
         <v>10.406166666666666</v>
       </c>
     </row>
@@ -1266,7 +2365,7 @@
       </c>
       <c r="M25" s="1"/>
       <c r="N25">
-        <f t="shared" ref="N24:N41" si="11">AVERAGE(J25:L25)</f>
+        <f t="shared" ref="N25:N26" si="11">AVERAGE(J25:L25)</f>
         <v>0.43973333333333331</v>
       </c>
     </row>
@@ -1382,7 +2481,7 @@
       </c>
       <c r="M29" s="1"/>
       <c r="N29">
-        <f t="shared" ref="N29:N41" si="12">AVERAGE(J29:L29)</f>
+        <f t="shared" ref="N29:N31" si="12">AVERAGE(J29:L29)</f>
         <v>10.004800000000001</v>
       </c>
     </row>
@@ -1564,7 +2663,7 @@
       </c>
       <c r="M35" s="1"/>
       <c r="N35">
-        <f t="shared" ref="N34:N41" si="13">AVERAGE(J35:L35)</f>
+        <f t="shared" ref="N35:N36" si="13">AVERAGE(J35:L35)</f>
         <v>0.49656666666666666</v>
       </c>
     </row>

</xml_diff>